<commit_message>
Map for symbionts - updated with gradient for latitude
</commit_message>
<xml_diff>
--- a/Map/Symbiont.coords.xlsx
+++ b/Map/Symbiont.coords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myjcuedu-my.sharepoint.com/personal/magena_marzonie_my_jcu_edu_au/Documents/R Scripts/Symbionts_CSMP/Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F70DDD94-E5C7-2044-A4E3-AEFEAEC82CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{F70DDD94-E5C7-2044-A4E3-AEFEAEC82CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C5DEDAD-9278-3D48-BC8B-911B1BA50CEE}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="940" windowWidth="27640" windowHeight="16940" xr2:uid="{FC4CFE1E-80EF-1945-BCD6-147A3885F940}"/>
+    <workbookView xWindow="-35340" yWindow="2320" windowWidth="27640" windowHeight="16940" xr2:uid="{FC4CFE1E-80EF-1945-BCD6-147A3885F940}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,12 +40,6 @@
     <t>Reef</t>
   </si>
   <si>
-    <t>GPS south</t>
-  </si>
-  <si>
-    <t>GPS east</t>
-  </si>
-  <si>
     <t>Bougainville</t>
   </si>
   <si>
@@ -83,6 +77,12 @@
   </si>
   <si>
     <t>Wreck</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,15 +463,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>15.50667</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>16.9315</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>17.702179999999998</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>21.010429999999999</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>16.943480000000001</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>16.526129999999998</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>17.59065</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>19.12125</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>15.97315</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>13.88078</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>21.9178</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>16.287279999999999</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>22.19267</v>

</xml_diff>